<commit_message>
updates to sim and plotter
</commit_message>
<xml_diff>
--- a/tests/data/common species.xlsx
+++ b/tests/data/common species.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mulvihcr/PycharmProjects/pythonProject/msi/tests/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mulvihcr/PycharmProjects/pythonProject/mechsimulator/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{716E495C-1D40-EB4F-B4E5-385CC6083EBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC3CC4B3-DA9C-0849-9EC5-80B0F59EC6D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17680" yWindow="2080" windowWidth="26040" windowHeight="14940" xr2:uid="{82B23897-C4B1-6444-AFCE-BBDEB95A07E1}"/>
+    <workbookView xWindow="17720" yWindow="660" windowWidth="16480" windowHeight="13260" xr2:uid="{82B23897-C4B1-6444-AFCE-BBDEB95A07E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
   <si>
     <t>name</t>
   </si>
@@ -94,6 +94,39 @@
   </si>
   <si>
     <t>N2</t>
+  </si>
+  <si>
+    <t>spc</t>
+  </si>
+  <si>
+    <t>this column is here so I can copy paste easily</t>
+  </si>
+  <si>
+    <t>N#N</t>
+  </si>
+  <si>
+    <t>H2O</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>[H][H]</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>[N]=O</t>
+  </si>
+  <si>
+    <t>NO2</t>
+  </si>
+  <si>
+    <t>N(=O)[O]</t>
   </si>
 </sst>
 </file>
@@ -459,173 +492,295 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{704339FD-2BCA-C244-AA3F-70536EA1C429}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="38.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2">
-        <v>1</v>
-      </c>
       <c r="D2" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>3</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
       <c r="E4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>2</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
       <c r="E5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>12</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>2</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
       <c r="E6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>15</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>2</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
       <c r="E7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>15</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>2</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
       <c r="E8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
         <v>17</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>18</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
       <c r="D9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
         <v>19</v>
       </c>
-      <c r="C10">
-        <v>1</v>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>